<commit_message>
Add Goal module with controller, model, migration, factory, and router
</commit_message>
<xml_diff>
--- a/src/statics/template.xlsx
+++ b/src/statics/template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Funval-WorkSpace\Sys\hs-app\src\statics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA5CA6F-EF78-4370-AFFA-2D74FE6071E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E553CDE-1D4F-4993-98C6-C62E101F8995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A7544D1-2258-47FF-84AE-E9936A2337CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$M$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -235,6 +235,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -243,12 +249,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -704,26 +704,26 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="4"/>
       <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="4"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="10"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="4"/>
       <c r="F2" s="8" t="s">
         <v>17</v>
@@ -733,16 +733,16 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="10"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="25.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="4"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="4"/>
       <c r="F3" s="8" t="s">
         <v>18</v>
@@ -752,7 +752,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="12"/>
       <c r="M3" s="4"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -776,29 +776,29 @@
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="12"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="12"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="12"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
@@ -832,15 +832,15 @@
         <v>3</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="12"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="12"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -849,15 +849,15 @@
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="12"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -866,28 +866,28 @@
         <v>5</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="12"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="12"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
@@ -909,41 +909,41 @@
         <v>7</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="12"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="12"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="12"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="12"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
@@ -965,44 +965,44 @@
         <v>10</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="12"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="12"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="12"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="12"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="12"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="12"/>
+      <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
@@ -1024,30 +1024,30 @@
         <v>13</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="12"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="12"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="12"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="12"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="9"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="12"/>
+      <c r="L24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>